<commit_message>
saving SEM image progress
</commit_message>
<xml_diff>
--- a/01-data/column_rename_mapping.xlsx
+++ b/01-data/column_rename_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danramirez/mbs-structural-equation-modeling/01-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1989623-D400-A94D-B52F-8ECFAC026AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ACABD1-F3ED-AE4B-871F-476E18D1780C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="500" windowWidth="27640" windowHeight="15860" activeTab="1" xr2:uid="{05942F46-CA0F-F744-9F7B-FB5E37380A0B}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15860" activeTab="1" xr2:uid="{05942F46-CA0F-F744-9F7B-FB5E37380A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -1559,12 +1559,6 @@
     <t>Xvar_gender</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Xvar_politics</t>
   </si>
   <si>
@@ -1578,6 +1572,12 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1999,9 +1999,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2014,7 +2011,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2352,10 +2348,10 @@
   <dimension ref="A1:B233"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B212" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A233" sqref="A233"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4225,15 +4221,10 @@
         <v>360</v>
       </c>
       <c r="B233" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B231" xr:uid="{C5CCC31B-3E15-5849-A807-1419182007A1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B231">
-      <sortCondition ref="B1:B231"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4242,14 +4233,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE7EF21-2F33-1340-9D4E-5B996CEF251E}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -4980,7 +4971,7 @@
       <c r="C41" s="32">
         <v>3</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" t="s">
         <v>437</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -4994,7 +4985,7 @@
       <c r="B42" s="31">
         <v>1</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="45" t="s">
         <v>473</v>
       </c>
       <c r="D42" s="1"/>
@@ -5007,7 +4998,7 @@
       <c r="B43" s="31">
         <v>2</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D43" s="3"/>
@@ -5020,7 +5011,7 @@
       <c r="B44" s="31">
         <v>8</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D44" s="3"/>
@@ -5033,7 +5024,7 @@
       <c r="B45" s="32">
         <v>9</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="46" t="s">
         <v>474</v>
       </c>
       <c r="D45" s="3"/>
@@ -5046,7 +5037,7 @@
       <c r="B46" s="30">
         <v>1</v>
       </c>
-      <c r="C46" s="48" t="s">
+      <c r="C46" s="47" t="s">
         <v>473</v>
       </c>
       <c r="D46" s="3"/>
@@ -5060,7 +5051,7 @@
       <c r="B47" s="31">
         <v>2</v>
       </c>
-      <c r="C47" s="46" t="s">
+      <c r="C47" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D47" s="3"/>
@@ -5074,7 +5065,7 @@
       <c r="B48" s="31">
         <v>8</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D48" s="3"/>
@@ -5088,7 +5079,7 @@
       <c r="B49" s="32">
         <v>9</v>
       </c>
-      <c r="C49" s="47" t="s">
+      <c r="C49" s="46" t="s">
         <v>474</v>
       </c>
       <c r="D49" s="3"/>
@@ -5102,7 +5093,7 @@
       <c r="B50" s="30">
         <v>1</v>
       </c>
-      <c r="C50" s="48" t="s">
+      <c r="C50" s="47" t="s">
         <v>473</v>
       </c>
       <c r="D50" s="3"/>
@@ -5115,7 +5106,7 @@
       <c r="B51" s="31">
         <v>2</v>
       </c>
-      <c r="C51" s="46" t="s">
+      <c r="C51" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D51" s="3"/>
@@ -5128,7 +5119,7 @@
       <c r="B52" s="31">
         <v>8</v>
       </c>
-      <c r="C52" s="46" t="s">
+      <c r="C52" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D52" s="3"/>
@@ -5141,7 +5132,7 @@
       <c r="B53" s="32">
         <v>9</v>
       </c>
-      <c r="C53" s="47" t="s">
+      <c r="C53" s="46" t="s">
         <v>474</v>
       </c>
       <c r="D53" s="3"/>
@@ -5154,7 +5145,7 @@
       <c r="B54" s="30">
         <v>1</v>
       </c>
-      <c r="C54" s="48" t="s">
+      <c r="C54" s="47" t="s">
         <v>473</v>
       </c>
       <c r="D54" s="3"/>
@@ -5167,7 +5158,7 @@
       <c r="B55" s="31">
         <v>2</v>
       </c>
-      <c r="C55" s="46" t="s">
+      <c r="C55" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D55" s="3"/>
@@ -5180,7 +5171,7 @@
       <c r="B56" s="31">
         <v>8</v>
       </c>
-      <c r="C56" s="46" t="s">
+      <c r="C56" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D56" s="3"/>
@@ -5193,7 +5184,7 @@
       <c r="B57" s="32">
         <v>9</v>
       </c>
-      <c r="C57" s="47" t="s">
+      <c r="C57" s="46" t="s">
         <v>474</v>
       </c>
       <c r="D57" s="3"/>
@@ -5206,7 +5197,7 @@
       <c r="B58" s="30">
         <v>1</v>
       </c>
-      <c r="C58" s="48" t="s">
+      <c r="C58" s="47" t="s">
         <v>473</v>
       </c>
       <c r="D58" s="3"/>
@@ -5219,7 +5210,7 @@
       <c r="B59" s="31">
         <v>2</v>
       </c>
-      <c r="C59" s="46" t="s">
+      <c r="C59" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D59" s="3"/>
@@ -5232,7 +5223,7 @@
       <c r="B60" s="31">
         <v>8</v>
       </c>
-      <c r="C60" s="46" t="s">
+      <c r="C60" s="45" t="s">
         <v>474</v>
       </c>
       <c r="D60" s="3"/>
@@ -5245,7 +5236,7 @@
       <c r="B61" s="32">
         <v>9</v>
       </c>
-      <c r="C61" s="47" t="s">
+      <c r="C61" s="46" t="s">
         <v>474</v>
       </c>
       <c r="D61" s="3"/>
@@ -5259,7 +5250,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
@@ -5268,102 +5259,102 @@
       <c r="A63" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="B63" s="32">
+      <c r="B63" s="31">
         <v>2</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B64" s="41">
         <v>1</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="B65" s="44">
+        <v>2</v>
+      </c>
+      <c r="C65" s="33" t="s">
         <v>507</v>
-      </c>
-      <c r="B65" s="45">
-        <v>2</v>
-      </c>
-      <c r="C65" s="44" t="s">
-        <v>509</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="B66" s="45">
+        <v>505</v>
+      </c>
+      <c r="B66" s="44">
         <v>3</v>
       </c>
-      <c r="C66" s="44" t="s">
-        <v>510</v>
+      <c r="C66" s="33" t="s">
+        <v>508</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="B67" s="45">
+        <v>505</v>
+      </c>
+      <c r="B67" s="44">
         <v>4</v>
       </c>
-      <c r="C67" s="44" t="s">
-        <v>511</v>
+      <c r="C67" s="33" t="s">
+        <v>509</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="B68" s="45">
+        <v>505</v>
+      </c>
+      <c r="B68" s="44">
         <v>5</v>
       </c>
-      <c r="C68" s="44" t="s">
-        <v>511</v>
+      <c r="C68" s="33" t="s">
+        <v>509</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="B69" s="45">
+        <v>505</v>
+      </c>
+      <c r="B69" s="44">
         <v>8</v>
       </c>
-      <c r="C69" s="44" t="s">
-        <v>511</v>
+      <c r="C69" s="33" t="s">
+        <v>509</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B70" s="43">
         <v>9</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="6"/>

</xml_diff>